<commit_message>
add fouling and sampling event draft spreadsheets
</commit_message>
<xml_diff>
--- a/resources/data_entry_spreadsheet_glossary_template.xlsx
+++ b/resources/data_entry_spreadsheet_glossary_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6C41DD5-9070-44F0-9DE0-57C882080895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43876C7-4713-419A-8911-D9BC18E05EC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="2565" windowWidth="21600" windowHeight="11505" xr2:uid="{87084C07-6C93-4E0B-8172-15FBCF2A707E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{87084C07-6C93-4E0B-8172-15FBCF2A707E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
   <si>
     <t>protocol_name</t>
   </si>
@@ -57,6 +57,93 @@
   </si>
   <si>
     <t>field_sheet_notes</t>
+  </si>
+  <si>
+    <t>Sampling Event Protocol</t>
+  </si>
+  <si>
+    <t>site metadata</t>
+  </si>
+  <si>
+    <t>site_code</t>
+  </si>
+  <si>
+    <t>location_name</t>
+  </si>
+  <si>
+    <t>sample_collection_year</t>
+  </si>
+  <si>
+    <t>sample_collection_month</t>
+  </si>
+  <si>
+    <t>sample_collection_day</t>
+  </si>
+  <si>
+    <t>visibility_m</t>
+  </si>
+  <si>
+    <t>habitat_type</t>
+  </si>
+  <si>
+    <t>sample_event_personnel</t>
+  </si>
+  <si>
+    <t>photo_filename</t>
+  </si>
+  <si>
+    <t>photo_location</t>
+  </si>
+  <si>
+    <t>photo_direction</t>
+  </si>
+  <si>
+    <t>camera_used</t>
+  </si>
+  <si>
+    <t>photographer</t>
+  </si>
+  <si>
+    <t>logger_id</t>
+  </si>
+  <si>
+    <t>deployment_location</t>
+  </si>
+  <si>
+    <t>logger_deployment_notes</t>
+  </si>
+  <si>
+    <t>logger deployment</t>
+  </si>
+  <si>
+    <t>transect metadata</t>
+  </si>
+  <si>
+    <t>transect</t>
+  </si>
+  <si>
+    <t>depth_min_m</t>
+  </si>
+  <si>
+    <t>depth_max_m</t>
+  </si>
+  <si>
+    <t>transect_notes</t>
+  </si>
+  <si>
+    <t>site_notes</t>
+  </si>
+  <si>
+    <t>transect_begin_decimal_latitude</t>
+  </si>
+  <si>
+    <t>transect_begin_decimal_longitude</t>
+  </si>
+  <si>
+    <t>transect_end_decimal_latitude</t>
+  </si>
+  <si>
+    <t>transect_end_decimal_longitude</t>
   </si>
 </sst>
 </file>
@@ -94,9 +181,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,17 +496,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB314508-5C86-4A11-9916-394451C7F414}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
     <col min="6" max="7" width="12.42578125" style="1" customWidth="1"/>
@@ -455,6 +540,391 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>